<commit_message>
restAPI update for file path
</commit_message>
<xml_diff>
--- a/check.xlsx
+++ b/check.xlsx
@@ -1,67 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27510"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/raghupathynarayanamoorthy/Desktop/fabrikProject/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="460" windowWidth="16100" windowHeight="9660"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="9660" windowWidth="16100" xWindow="240" yWindow="460"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <definedNames/>
+  <calcPr calcId="0" concurrentCalc="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t>Long</t>
-  </si>
-  <si>
-    <t>Short</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="2">
+    <numFmt formatCode="YYYY-MM-DD" numFmtId="164"/>
+    <numFmt formatCode="yyyy-mm-dd" numFmtId="165"/>
+  </numFmts>
+  <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -90,25 +67,21 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="5">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="164" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -396,32 +369,92 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="57" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25" style="2" bestFit="1" customWidth="1"/>
+    <col customWidth="1" max="1" min="1" style="2" width="17.83203125"/>
+    <col bestFit="1" customWidth="1" max="2" min="2" style="2" width="57"/>
+    <col bestFit="1" customWidth="1" max="3" min="3" style="2" width="25"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>Date</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>Long</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Short</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="4" t="n">
+        <v>43806</v>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>https://www.google.com/search?ei=fRZjXOTcNoOYafn9rKgG</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="4" t="n">
+        <v>43806</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>https://www.youtube.com/watch?v=zA0eqkqwaKE</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="n">
+        <v>43806</v>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>https://olympus.greatlearning.in/login</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>http://127.0.0.1:5000/cV63QT</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="4" t="n">
+        <v>43806</v>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>https://zoom.us/wc/leave?meetingNumber=442013660</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>http://127.0.0.1:5000/shxMzb</t>
+        </is>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>